<commit_message>
ajustando layout... lorofacil simulador
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt.xlsx
+++ b/LoteriasExcel/Lotofacil_edt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22D937B9-2ED2-4F16-A349-4208ACA3E468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC84868-1D46-4AD7-B9E6-6A68BB8C541E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62190" yWindow="1095" windowWidth="30015" windowHeight="14055" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="59940" yWindow="6120" windowWidth="29520" windowHeight="12135" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P301"/>
+  <dimension ref="A1:P307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="A301" sqref="A301:XFD301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -15513,21 +15513,312 @@
         <v>24</v>
       </c>
     </row>
+    <row r="302" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A302">
+        <v>3466</v>
+      </c>
+      <c r="B302">
+        <v>1</v>
+      </c>
+      <c r="C302">
+        <v>5</v>
+      </c>
+      <c r="D302">
+        <v>6</v>
+      </c>
+      <c r="E302">
+        <v>7</v>
+      </c>
+      <c r="F302">
+        <v>9</v>
+      </c>
+      <c r="G302">
+        <v>10</v>
+      </c>
+      <c r="H302">
+        <v>12</v>
+      </c>
+      <c r="I302">
+        <v>15</v>
+      </c>
+      <c r="J302">
+        <v>17</v>
+      </c>
+      <c r="K302">
+        <v>18</v>
+      </c>
+      <c r="L302">
+        <v>19</v>
+      </c>
+      <c r="M302">
+        <v>21</v>
+      </c>
+      <c r="N302">
+        <v>23</v>
+      </c>
+      <c r="O302">
+        <v>24</v>
+      </c>
+      <c r="P302">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="303" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A303">
+        <v>3467</v>
+      </c>
+      <c r="B303">
+        <v>3</v>
+      </c>
+      <c r="C303">
+        <v>4</v>
+      </c>
+      <c r="D303">
+        <v>5</v>
+      </c>
+      <c r="E303">
+        <v>6</v>
+      </c>
+      <c r="F303">
+        <v>7</v>
+      </c>
+      <c r="G303">
+        <v>8</v>
+      </c>
+      <c r="H303">
+        <v>9</v>
+      </c>
+      <c r="I303">
+        <v>13</v>
+      </c>
+      <c r="J303">
+        <v>14</v>
+      </c>
+      <c r="K303">
+        <v>16</v>
+      </c>
+      <c r="L303">
+        <v>18</v>
+      </c>
+      <c r="M303">
+        <v>19</v>
+      </c>
+      <c r="N303">
+        <v>20</v>
+      </c>
+      <c r="O303">
+        <v>21</v>
+      </c>
+      <c r="P303">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="304" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A304">
+        <v>3468</v>
+      </c>
+      <c r="B304">
+        <v>1</v>
+      </c>
+      <c r="C304">
+        <v>3</v>
+      </c>
+      <c r="D304">
+        <v>4</v>
+      </c>
+      <c r="E304">
+        <v>6</v>
+      </c>
+      <c r="F304">
+        <v>9</v>
+      </c>
+      <c r="G304">
+        <v>10</v>
+      </c>
+      <c r="H304">
+        <v>12</v>
+      </c>
+      <c r="I304">
+        <v>13</v>
+      </c>
+      <c r="J304">
+        <v>14</v>
+      </c>
+      <c r="K304">
+        <v>18</v>
+      </c>
+      <c r="L304">
+        <v>19</v>
+      </c>
+      <c r="M304">
+        <v>21</v>
+      </c>
+      <c r="N304">
+        <v>23</v>
+      </c>
+      <c r="O304">
+        <v>24</v>
+      </c>
+      <c r="P304">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="305" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A305">
+        <v>3469</v>
+      </c>
+      <c r="B305">
+        <v>1</v>
+      </c>
+      <c r="C305">
+        <v>3</v>
+      </c>
+      <c r="D305">
+        <v>5</v>
+      </c>
+      <c r="E305">
+        <v>6</v>
+      </c>
+      <c r="F305">
+        <v>7</v>
+      </c>
+      <c r="G305">
+        <v>8</v>
+      </c>
+      <c r="H305">
+        <v>11</v>
+      </c>
+      <c r="I305">
+        <v>12</v>
+      </c>
+      <c r="J305">
+        <v>13</v>
+      </c>
+      <c r="K305">
+        <v>15</v>
+      </c>
+      <c r="L305">
+        <v>17</v>
+      </c>
+      <c r="M305">
+        <v>18</v>
+      </c>
+      <c r="N305">
+        <v>21</v>
+      </c>
+      <c r="O305">
+        <v>22</v>
+      </c>
+      <c r="P305">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="306" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A306">
+        <v>3470</v>
+      </c>
+      <c r="B306">
+        <v>1</v>
+      </c>
+      <c r="C306">
+        <v>4</v>
+      </c>
+      <c r="D306">
+        <v>5</v>
+      </c>
+      <c r="E306">
+        <v>7</v>
+      </c>
+      <c r="F306">
+        <v>8</v>
+      </c>
+      <c r="G306">
+        <v>10</v>
+      </c>
+      <c r="H306">
+        <v>12</v>
+      </c>
+      <c r="I306">
+        <v>13</v>
+      </c>
+      <c r="J306">
+        <v>14</v>
+      </c>
+      <c r="K306">
+        <v>18</v>
+      </c>
+      <c r="L306">
+        <v>20</v>
+      </c>
+      <c r="M306">
+        <v>21</v>
+      </c>
+      <c r="N306">
+        <v>22</v>
+      </c>
+      <c r="O306">
+        <v>23</v>
+      </c>
+      <c r="P306">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="307" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A307">
+        <v>3471</v>
+      </c>
+      <c r="B307">
+        <v>1</v>
+      </c>
+      <c r="C307">
+        <v>2</v>
+      </c>
+      <c r="D307">
+        <v>3</v>
+      </c>
+      <c r="E307">
+        <v>5</v>
+      </c>
+      <c r="F307">
+        <v>6</v>
+      </c>
+      <c r="G307">
+        <v>11</v>
+      </c>
+      <c r="H307">
+        <v>13</v>
+      </c>
+      <c r="I307">
+        <v>16</v>
+      </c>
+      <c r="J307">
+        <v>17</v>
+      </c>
+      <c r="K307">
+        <v>19</v>
+      </c>
+      <c r="L307">
+        <v>21</v>
+      </c>
+      <c r="M307">
+        <v>22</v>
+      </c>
+      <c r="N307">
+        <v>23</v>
+      </c>
+      <c r="O307">
+        <v>24</v>
+      </c>
+      <c r="P307">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15695,6 +15986,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -15706,14 +16006,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15733,6 +16025,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Ajustando funcionalidaade do modal Gera poastas premuium lotofacil
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt.xlsx
+++ b/LoteriasExcel/Lotofacil_edt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC84868-1D46-4AD7-B9E6-6A68BB8C541E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979161A8-AFA3-493E-B770-8200D39F8DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59940" yWindow="6120" windowWidth="29520" windowHeight="12135" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="65385" yWindow="615" windowWidth="25005" windowHeight="10515" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P307"/>
+  <dimension ref="A1:P308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
-      <selection activeCell="A301" sqref="A301:XFD301"/>
+    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
+      <selection activeCell="A308" sqref="A308:XFD308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -15813,12 +15813,71 @@
         <v>25</v>
       </c>
     </row>
+    <row r="308" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A308">
+        <v>3472</v>
+      </c>
+      <c r="B308">
+        <v>2</v>
+      </c>
+      <c r="C308">
+        <v>3</v>
+      </c>
+      <c r="D308">
+        <v>5</v>
+      </c>
+      <c r="E308">
+        <v>7</v>
+      </c>
+      <c r="F308">
+        <v>10</v>
+      </c>
+      <c r="G308">
+        <v>11</v>
+      </c>
+      <c r="H308">
+        <v>12</v>
+      </c>
+      <c r="I308">
+        <v>13</v>
+      </c>
+      <c r="J308">
+        <v>15</v>
+      </c>
+      <c r="K308">
+        <v>18</v>
+      </c>
+      <c r="L308">
+        <v>19</v>
+      </c>
+      <c r="M308">
+        <v>21</v>
+      </c>
+      <c r="N308">
+        <v>23</v>
+      </c>
+      <c r="O308">
+        <v>24</v>
+      </c>
+      <c r="P308">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15986,15 +16045,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -16006,6 +16056,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16025,14 +16083,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>

</xml_diff>